<commit_message>
Arrowhead - update to handle text notes, MissionControl - refactor for all post methods, logging embedded.
</commit_message>
<xml_diff>
--- a/Sheet Manager/src/Archive/HOK.SheetManager_Excel/SheetMakerData_Test.xlsx
+++ b/Sheet Manager/src/Archive/HOK.SheetManager_Excel/SheetMakerData_Test.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konrad.sobon\OneDrive - HOK\GoogleDrive\Work\HOK-Revit-Addins\Sheet Manager\src\Archive\HOK.SheetManager_Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="19440" windowHeight="12210"/>
   </bookViews>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="669">
   <si>
     <t>Sheet Number</t>
   </si>
@@ -2030,6 +2035,9 @@
   </si>
   <si>
     <t>CEILING DETAIL - TYPICAL ACT SUSPENSION DETAIL</t>
+  </si>
+  <si>
+    <t>PLUMBING FLOOR PLAN - LEVEL 1</t>
   </si>
 </sst>
 </file>
@@ -2076,6 +2084,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2124,7 +2135,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2159,7 +2170,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2371,7 +2382,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2429,7 +2440,7 @@
         <v>265</v>
       </c>
       <c r="B3" t="s">
-        <v>266</v>
+        <v>668</v>
       </c>
       <c r="C3" t="s">
         <v>193</v>

</xml_diff>